<commit_message>
Add mono icon, add offset api
</commit_message>
<xml_diff>
--- a/cryws.3.27.xlsx
+++ b/cryws.3.27.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="63">
   <si>
     <t>api/coins</t>
   </si>
@@ -39,9 +39,6 @@
   </si>
   <si>
     <t>DELETE</t>
-  </si>
-  <si>
-    <t>api/tokens</t>
   </si>
   <si>
     <t>api/accounts</t>
@@ -423,7 +420,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -529,10 +526,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -544,37 +541,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -715,19 +682,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="medium">
@@ -790,199 +744,222 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1471,696 +1448,680 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.77734375" customWidth="1"/>
-    <col min="2" max="2" width="11.77734375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" style="4" customWidth="1"/>
     <col min="3" max="3" width="27.6640625" customWidth="1"/>
     <col min="4" max="4" width="51.5546875" customWidth="1"/>
-    <col min="5" max="5" width="19.109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="13.88671875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="14.77734375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="14.44140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="14.77734375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" style="3" customWidth="1"/>
     <col min="9" max="9" width="43.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="46.2" x14ac:dyDescent="0.85">
-      <c r="A1" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
+      <c r="A1" s="54" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
     </row>
     <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
+      <c r="A2" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+    </row>
+    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-    </row>
-    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="75" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
     </row>
     <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A6" s="49" t="s">
+      <c r="A6" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="55" t="s">
+      <c r="C6" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="55" t="s">
+      <c r="E6" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="45"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="40"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" s="40"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="55" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="57" t="s">
+      <c r="E8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="15">
+        <v>200</v>
+      </c>
+      <c r="G8" s="16">
+        <v>422</v>
+      </c>
+      <c r="H8" s="17"/>
+      <c r="I8" s="18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="52"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="11">
+        <v>200</v>
+      </c>
+      <c r="G9" s="12">
+        <v>422</v>
+      </c>
+      <c r="H9" s="14"/>
+      <c r="I9" s="24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="52"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="27">
+        <v>200</v>
+      </c>
+      <c r="G10" s="28">
+        <v>422</v>
+      </c>
+      <c r="H10" s="29"/>
+      <c r="I10" s="30" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="52"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="27">
+        <v>200</v>
+      </c>
+      <c r="G11" s="28">
+        <v>422</v>
+      </c>
+      <c r="H11" s="29"/>
+      <c r="I11" s="30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="52"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="33">
+        <v>200</v>
+      </c>
+      <c r="G12" s="33">
+        <v>422</v>
+      </c>
+      <c r="H12" s="33"/>
+      <c r="I12" s="34" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="52"/>
+      <c r="B13" s="41" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="52" t="s">
-        <v>42</v>
-      </c>
-      <c r="G6" s="53"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="49" t="s">
+      <c r="F13" s="11">
+        <v>200</v>
+      </c>
+      <c r="G13" s="12">
+        <v>422</v>
+      </c>
+      <c r="H13" s="14">
+        <v>401</v>
+      </c>
+      <c r="I13" s="19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="52"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="10">
+        <v>200</v>
+      </c>
+      <c r="G14" s="12">
+        <v>422</v>
+      </c>
+      <c r="H14" s="13">
+        <v>401</v>
+      </c>
+      <c r="I14" s="19"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="52"/>
+      <c r="B15" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="19"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="52"/>
+      <c r="B16" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="56" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="56" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="57" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="68">
+        <v>200</v>
+      </c>
+      <c r="G16" s="58">
+        <v>422</v>
+      </c>
+      <c r="H16" s="69">
+        <v>401</v>
+      </c>
+      <c r="I16" s="70" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="50"/>
-      <c r="B7" s="56"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="I7" s="50"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="13" t="s">
+      <c r="E17" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="11">
+        <v>200</v>
+      </c>
+      <c r="G17" s="72">
+        <v>422</v>
+      </c>
+      <c r="H17" s="14">
+        <v>401</v>
+      </c>
+      <c r="I17" s="35" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="71"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="11">
+        <v>200</v>
+      </c>
+      <c r="G18" s="12">
+        <v>422</v>
+      </c>
+      <c r="H18" s="14">
+        <v>401</v>
+      </c>
+      <c r="I18" s="35" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="71"/>
+      <c r="B19" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="10">
+        <v>200</v>
+      </c>
+      <c r="G19" s="12">
+        <v>422</v>
+      </c>
+      <c r="H19" s="13">
+        <v>401</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="71"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="11">
+        <v>200</v>
+      </c>
+      <c r="G20" s="12">
+        <v>422</v>
+      </c>
+      <c r="H20" s="14">
+        <v>401</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="71"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F21" s="11">
+        <v>200</v>
+      </c>
+      <c r="G21" s="12">
+        <v>422</v>
+      </c>
+      <c r="H21" s="14">
+        <v>401</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="71"/>
+      <c r="B22" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="10">
+        <v>200</v>
+      </c>
+      <c r="G22" s="12">
+        <v>422</v>
+      </c>
+      <c r="H22" s="13">
+        <v>401</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="71"/>
+      <c r="B23" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" s="11">
+        <v>200</v>
+      </c>
+      <c r="G23" s="12">
+        <v>422</v>
+      </c>
+      <c r="H23" s="14">
+        <v>401</v>
+      </c>
+      <c r="I23" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="21">
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="71"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="11">
         <v>200</v>
       </c>
-      <c r="G8" s="22">
+      <c r="G24" s="12">
         <v>422</v>
       </c>
-      <c r="H8" s="23"/>
-      <c r="I8" s="24" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="42"/>
-      <c r="B9" s="51"/>
-      <c r="C9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="17">
-        <v>200</v>
-      </c>
-      <c r="G9" s="18">
-        <v>422</v>
-      </c>
-      <c r="H9" s="20"/>
-      <c r="I9" s="60" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="42"/>
-      <c r="B10" s="51"/>
-      <c r="C10" s="61" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="61" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="62" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="63">
-        <v>200</v>
-      </c>
-      <c r="G10" s="64">
-        <v>422</v>
-      </c>
-      <c r="H10" s="65"/>
-      <c r="I10" s="66" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="42"/>
-      <c r="B11" s="51"/>
-      <c r="C11" s="61" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="61" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" s="62" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="63">
-        <v>200</v>
-      </c>
-      <c r="G11" s="64">
-        <v>422</v>
-      </c>
-      <c r="H11" s="65"/>
-      <c r="I11" s="66" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="42"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="67" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="67" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" s="68" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="69">
-        <v>200</v>
-      </c>
-      <c r="G12" s="69">
-        <v>422</v>
-      </c>
-      <c r="H12" s="69"/>
-      <c r="I12" s="70" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="42"/>
-      <c r="B13" s="40" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="17">
-        <v>200</v>
-      </c>
-      <c r="G13" s="18">
-        <v>422</v>
-      </c>
-      <c r="H13" s="20">
+      <c r="H24" s="14">
         <v>401</v>
       </c>
-      <c r="I13" s="25" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="42"/>
-      <c r="B14" s="39"/>
-      <c r="C14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="16">
-        <v>200</v>
-      </c>
-      <c r="G14" s="18">
-        <v>422</v>
-      </c>
-      <c r="H14" s="19">
-        <v>401</v>
-      </c>
-      <c r="I14" s="25"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="42"/>
-      <c r="B15" s="34" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="72" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="25"/>
-    </row>
-    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="43"/>
-      <c r="B16" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="F16" s="26">
-        <v>200</v>
-      </c>
-      <c r="G16" s="27">
-        <v>422</v>
-      </c>
-      <c r="H16" s="28">
-        <v>401</v>
-      </c>
-      <c r="I16" s="29" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="71" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="F17" s="21">
-        <v>200</v>
-      </c>
-      <c r="G17" s="22">
-        <v>422</v>
-      </c>
-      <c r="H17" s="23">
-        <v>401</v>
-      </c>
-      <c r="I17" s="73" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="45"/>
-      <c r="B18" s="47"/>
-      <c r="C18" s="72" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F18" s="17">
-        <v>200</v>
-      </c>
-      <c r="G18" s="18">
-        <v>422</v>
-      </c>
-      <c r="H18" s="20">
-        <v>401</v>
-      </c>
-      <c r="I18" s="60" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="45"/>
-      <c r="B19" s="47" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="F19" s="16">
-        <v>200</v>
-      </c>
-      <c r="G19" s="18">
-        <v>422</v>
-      </c>
-      <c r="H19" s="19">
-        <v>401</v>
-      </c>
-      <c r="I19" s="30" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="45"/>
-      <c r="B20" s="47"/>
-      <c r="C20" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F20" s="17">
-        <v>200</v>
-      </c>
-      <c r="G20" s="18">
-        <v>422</v>
-      </c>
-      <c r="H20" s="20">
-        <v>401</v>
-      </c>
-      <c r="I20" s="30" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="45"/>
-      <c r="B21" s="47"/>
-      <c r="C21" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="F21" s="17">
-        <v>200</v>
-      </c>
-      <c r="G21" s="18">
-        <v>422</v>
-      </c>
-      <c r="H21" s="20">
-        <v>401</v>
-      </c>
-      <c r="I21" s="30" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="45"/>
-      <c r="B22" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F22" s="16">
-        <v>200</v>
-      </c>
-      <c r="G22" s="18">
-        <v>422</v>
-      </c>
-      <c r="H22" s="19">
-        <v>401</v>
-      </c>
-      <c r="I22" s="30" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="45"/>
-      <c r="B23" s="47" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="F23" s="17">
-        <v>200</v>
-      </c>
-      <c r="G23" s="18">
-        <v>422</v>
-      </c>
-      <c r="H23" s="20">
-        <v>401</v>
-      </c>
-      <c r="I23" s="30" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="46"/>
-      <c r="B24" s="48"/>
-      <c r="C24" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="D24" s="9" t="s">
+      <c r="I24" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E24" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F24" s="31">
-        <v>200</v>
-      </c>
-      <c r="G24" s="27">
-        <v>422</v>
-      </c>
-      <c r="H24" s="32">
-        <v>401</v>
-      </c>
-      <c r="I24" s="33" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25" s="72" t="s">
-        <v>53</v>
-      </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="23"/>
-      <c r="I25" s="24"/>
+      <c r="A25" s="59"/>
+      <c r="B25" s="60"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="62"/>
+      <c r="E25" s="63"/>
+      <c r="F25" s="64"/>
+      <c r="G25" s="65"/>
+      <c r="H25" s="66"/>
+      <c r="I25" s="62"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="42"/>
-      <c r="B26" s="39"/>
-      <c r="C26" s="72" t="s">
-        <v>53</v>
-      </c>
-      <c r="D26" s="1"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="25"/>
+      <c r="A26" s="59"/>
+      <c r="B26" s="60"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="63"/>
+      <c r="F26" s="64"/>
+      <c r="G26" s="65"/>
+      <c r="H26" s="66"/>
+      <c r="I26" s="62"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="42"/>
-      <c r="B27" s="40" t="s">
-        <v>2</v>
-      </c>
-      <c r="C27" s="72" t="s">
-        <v>53</v>
-      </c>
-      <c r="D27" s="1"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="25"/>
+      <c r="A27" s="59"/>
+      <c r="B27" s="60"/>
+      <c r="C27" s="61"/>
+      <c r="D27" s="62"/>
+      <c r="E27" s="63"/>
+      <c r="F27" s="64"/>
+      <c r="G27" s="65"/>
+      <c r="H27" s="66"/>
+      <c r="I27" s="62"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="42"/>
-      <c r="B28" s="39"/>
-      <c r="C28" s="72" t="s">
-        <v>53</v>
-      </c>
-      <c r="D28" s="1"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="25"/>
+      <c r="A28" s="59"/>
+      <c r="B28" s="60"/>
+      <c r="C28" s="61"/>
+      <c r="D28" s="62"/>
+      <c r="E28" s="63"/>
+      <c r="F28" s="64"/>
+      <c r="G28" s="65"/>
+      <c r="H28" s="66"/>
+      <c r="I28" s="62"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="42"/>
-      <c r="B29" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" s="72" t="s">
-        <v>53</v>
-      </c>
-      <c r="D29" s="1"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="25"/>
+      <c r="A29" s="59"/>
+      <c r="B29" s="60"/>
+      <c r="C29" s="61"/>
+      <c r="D29" s="62"/>
+      <c r="E29" s="63"/>
+      <c r="F29" s="64"/>
+      <c r="G29" s="65"/>
+      <c r="H29" s="66"/>
+      <c r="I29" s="62"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="42"/>
-      <c r="B30" s="51"/>
-      <c r="C30" s="72" t="s">
-        <v>53</v>
-      </c>
-      <c r="D30" s="1"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="25"/>
+      <c r="A30" s="59"/>
+      <c r="B30" s="60"/>
+      <c r="C30" s="61"/>
+      <c r="D30" s="62"/>
+      <c r="E30" s="63"/>
+      <c r="F30" s="64"/>
+      <c r="G30" s="65"/>
+      <c r="H30" s="66"/>
+      <c r="I30" s="62"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="42"/>
-      <c r="B31" s="51"/>
-      <c r="C31" s="72" t="s">
-        <v>53</v>
-      </c>
-      <c r="D31" s="1"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="25"/>
+      <c r="A31" s="59"/>
+      <c r="B31" s="60"/>
+      <c r="C31" s="61"/>
+      <c r="D31" s="62"/>
+      <c r="E31" s="63"/>
+      <c r="F31" s="64"/>
+      <c r="G31" s="65"/>
+      <c r="H31" s="66"/>
+      <c r="I31" s="62"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="42"/>
-      <c r="B32" s="51"/>
-      <c r="C32" s="72" t="s">
-        <v>53</v>
-      </c>
-      <c r="D32" s="1"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="25"/>
+      <c r="A32" s="59"/>
+      <c r="B32" s="60"/>
+      <c r="C32" s="61"/>
+      <c r="D32" s="62"/>
+      <c r="E32" s="63"/>
+      <c r="F32" s="64"/>
+      <c r="G32" s="65"/>
+      <c r="H32" s="66"/>
+      <c r="I32" s="62"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="42"/>
-      <c r="B33" s="51"/>
-      <c r="C33" s="72" t="s">
-        <v>53</v>
-      </c>
-      <c r="D33" s="1"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="25"/>
+      <c r="A33" s="59"/>
+      <c r="B33" s="60"/>
+      <c r="C33" s="61"/>
+      <c r="D33" s="62"/>
+      <c r="E33" s="63"/>
+      <c r="F33" s="64"/>
+      <c r="G33" s="65"/>
+      <c r="H33" s="66"/>
+      <c r="I33" s="62"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="42"/>
-      <c r="B34" s="39"/>
-      <c r="C34" s="72" t="s">
-        <v>53</v>
-      </c>
-      <c r="D34" s="1"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="18"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="25"/>
-    </row>
-    <row r="35" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="43"/>
-      <c r="B35" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35" s="72" t="s">
-        <v>53</v>
-      </c>
-      <c r="D35" s="8"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="31"/>
-      <c r="G35" s="27"/>
-      <c r="H35" s="32"/>
-      <c r="I35" s="29"/>
+      <c r="A34" s="59"/>
+      <c r="B34" s="60"/>
+      <c r="C34" s="61"/>
+      <c r="D34" s="62"/>
+      <c r="E34" s="63"/>
+      <c r="F34" s="64"/>
+      <c r="G34" s="65"/>
+      <c r="H34" s="66"/>
+      <c r="I34" s="62"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="59"/>
+      <c r="B35" s="67"/>
+      <c r="C35" s="61"/>
+      <c r="D35" s="62"/>
+      <c r="E35" s="63"/>
+      <c r="F35" s="64"/>
+      <c r="G35" s="65"/>
+      <c r="H35" s="66"/>
+      <c r="I35" s="62"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B36" s="67"/>
+      <c r="C36" s="62"/>
+      <c r="D36" s="62"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B37" s="67"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B38" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A8:A16"/>
     <mergeCell ref="A17:A24"/>
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="I6:I7"/>
@@ -2176,11 +2137,6 @@
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B17:B18"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A8:A16"/>
   </mergeCells>
   <conditionalFormatting sqref="B8:B12">
     <cfRule type="cellIs" dxfId="25" priority="27" operator="equal">

</xml_diff>